<commit_message>
feat: generate lists for work and rest dates
</commit_message>
<xml_diff>
--- a/work_and_rest_days.xlsx
+++ b/work_and_rest_days.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MEGA\projects\other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEGA\projects\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43052C3D-6325-4F55-ACAF-3DA384FA97AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23865" windowHeight="8190"/>
+    <workbookView xWindow="12540" yWindow="1188" windowWidth="10476" windowHeight="11004" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,17 +353,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -533,6 +534,20 @@
         <v>1973</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2023</v>
+      </c>
+      <c r="B13">
+        <v>247</v>
+      </c>
+      <c r="C13">
+        <v>118</v>
+      </c>
+      <c r="D13">
+        <v>1973</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>